<commit_message>
Updated placeholder environmental code
Updated placeholder environmental code. This code allows the model to run without needing the inputs from env.py.
</commit_message>
<xml_diff>
--- a/RESULTS_TOPSIS.xlsx
+++ b/RESULTS_TOPSIS.xlsx
@@ -485,13 +485,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.4169383501957792</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9202028148910231</v>
+        <v>0.6179412663638073</v>
       </c>
       <c r="E3" t="n">
-        <v>0.09485086445093371</v>
+        <v>0.2631158740604405</v>
       </c>
     </row>
     <row r="4">
@@ -504,13 +504,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0.4032894770784745</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1223938372247587</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8722654415707353</v>
+        <v>0.09385465034257801</v>
       </c>
     </row>
     <row r="5">
@@ -561,13 +561,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.6209799435389665</v>
+        <v>0.5258542493189475</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6149600267302531</v>
+        <v>0.7592750916259005</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3479029959509038</v>
+        <v>0.1539538788908697</v>
       </c>
     </row>
     <row r="8">
@@ -580,13 +580,13 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.5932977056435308</v>
+        <v>0.5093697533141097</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6175644845519238</v>
+        <v>0.7548668673553367</v>
       </c>
       <c r="E8" t="n">
-        <v>0.3468472602957524</v>
+        <v>0.1677684496388044</v>
       </c>
     </row>
     <row r="9">
@@ -599,13 +599,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.4998225055563112</v>
+        <v>0.5739394718338696</v>
       </c>
       <c r="D9" t="n">
-        <v>0.7367020903620679</v>
+        <v>0.7325124145915776</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2418927413780549</v>
+        <v>0.1760031839503879</v>
       </c>
     </row>
     <row r="10">
@@ -618,13 +618,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.7445704557824226</v>
+        <v>0.4350867014405913</v>
       </c>
       <c r="D10" t="n">
-        <v>0.4232527355986462</v>
+        <v>0.8691106329719475</v>
       </c>
       <c r="E10" t="n">
-        <v>0.5678951657537803</v>
+        <v>0.1124507382518814</v>
       </c>
     </row>
     <row r="11">
@@ -637,13 +637,13 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.5885034410239408</v>
+        <v>0.5537265071792478</v>
       </c>
       <c r="D11" t="n">
-        <v>0.7715551650937036</v>
+        <v>0.8509751868720293</v>
       </c>
       <c r="E11" t="n">
-        <v>0.2023530753408894</v>
+        <v>0.09081965925284612</v>
       </c>
     </row>
     <row r="12">
@@ -656,13 +656,13 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.7292805432515246</v>
+        <v>0.6584834330021733</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5111464247888471</v>
+        <v>0.5782207208179736</v>
       </c>
       <c r="E12" t="n">
-        <v>0.3573383098164276</v>
+        <v>0.2600230058648094</v>
       </c>
     </row>
   </sheetData>
@@ -735,10 +735,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
@@ -754,13 +754,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -811,10 +811,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
@@ -868,13 +868,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">

</xml_diff>